<commit_message>
update allowing dynamic number of stages. not tested
</commit_message>
<xml_diff>
--- a/src/data.xlsx
+++ b/src/data.xlsx
@@ -1,28 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanyoung/ryayoung/python-packages/tsopt/src/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C7FB63-7B44-9B47-9502-10220E48205E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="60160" yWindow="12260" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sensitivity Report 1"/>
-    <sheet r:id="rId2" sheetId="2" name="Main"/>
-    <sheet r:id="rId3" sheetId="3" name="cost1"/>
-    <sheet r:id="rId4" sheetId="4" name="cost2"/>
-    <sheet r:id="rId5" sheetId="5" name="capacity"/>
-    <sheet r:id="rId6" sheetId="6" name="demand"/>
+    <sheet name="Sensitivity Report 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="2" r:id="rId2"/>
+    <sheet name="cost1" sheetId="3" r:id="rId3"/>
+    <sheet name="cost2" sheetId="4" r:id="rId4"/>
+    <sheet name="capacity" sheetId="5" r:id="rId5"/>
+    <sheet name="demand" sheetId="6" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="1">'Elmore''s Ski Boots'!$C$16:$D$18,'Elmore''s Ski Boots'!$C$22:$G$23</definedName>
+    <definedName name="solver_adj" localSheetId="1">'[1]Elmore''s Ski Boots'!$C$16:$D$18,'[1]Elmore''s Ski Boots'!$C$22:$G$23</definedName>
     <definedName name="solver_cvg" localSheetId="1">0.0001</definedName>
     <definedName name="solver_drv">1</definedName>
     <definedName name="solver_eng">2</definedName>
     <definedName name="solver_itr">2147483647</definedName>
-    <definedName name="solver_lhs1">'Elmore''s Ski Boots'!$C$24:$G$24</definedName>
-    <definedName name="solver_lhs2">'Elmore''s Ski Boots'!$E$16:$E$18</definedName>
-    <definedName name="solver_lhs3">'Elmore''s Ski Boots'!$J$24:$J$25</definedName>
+    <definedName name="solver_lhs1">'[1]Elmore''s Ski Boots'!$C$24:$G$24</definedName>
+    <definedName name="solver_lhs2">'[1]Elmore''s Ski Boots'!$E$16:$E$18</definedName>
+    <definedName name="solver_lhs3">'[1]Elmore''s Ski Boots'!$J$24:$J$25</definedName>
     <definedName name="solver_lin">1</definedName>
     <definedName name="solver_mip">2147483647</definedName>
     <definedName name="solver_mni">30</definedName>
@@ -31,15 +40,15 @@
     <definedName name="solver_neg">1</definedName>
     <definedName name="solver_nod">2147483647</definedName>
     <definedName name="solver_num">3</definedName>
-    <definedName name="solver_opt">'Elmore''s Ski Boots'!$G$29</definedName>
+    <definedName name="solver_opt">'[1]Elmore''s Ski Boots'!$G$29</definedName>
     <definedName name="solver_pre">0.000001</definedName>
     <definedName name="solver_rbv">1</definedName>
     <definedName name="solver_rel1">3</definedName>
     <definedName name="solver_rel2">1</definedName>
     <definedName name="solver_rel3">2</definedName>
-    <definedName name="solver_rhs1">'Elmore''s Ski Boots'!$C$26:$G$26</definedName>
-    <definedName name="solver_rhs2">'Elmore''s Ski Boots'!$G$16:$G$18</definedName>
-    <definedName name="solver_rhs3">'Elmore''s Ski Boots'!$L$24:$L$25</definedName>
+    <definedName name="solver_rhs1">'[1]Elmore''s Ski Boots'!$C$26:$G$26</definedName>
+    <definedName name="solver_rhs2">'[1]Elmore''s Ski Boots'!$G$16:$G$18</definedName>
+    <definedName name="solver_rhs3">'[1]Elmore''s Ski Boots'!$L$24:$L$25</definedName>
     <definedName name="solver_rlx">1</definedName>
     <definedName name="solver_rsd">0</definedName>
     <definedName name="solver_scl">2</definedName>
@@ -51,7 +60,19 @@
     <definedName name="solver_val">0</definedName>
     <definedName name="solver_ver">2</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -370,8 +391,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,27 +449,27 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFb4c7e7"/>
+        <fgColor rgb="FFB4C7E7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffc000"/>
+        <fgColor rgb="FFFFC000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFc5e0b4"/>
+        <fgColor rgb="FFC5E0B4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70ad47"/>
+        <fgColor rgb="FF70AD47"/>
       </patternFill>
     </fill>
   </fills>
@@ -485,16 +505,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,133 +561,137 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Elmore's Ski Boots"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -675,10 +699,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -716,71 +740,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -808,7 +832,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -831,11 +855,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -844,13 +868,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -860,7 +884,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -869,7 +893,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -878,7 +902,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -886,10 +910,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -954,7 +978,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -962,19 +986,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="2.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="6.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="2.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.1640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>31</v>
       </c>
@@ -986,7 +1009,7 @@
       <c r="G1" s="25"/>
       <c r="H1" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>32</v>
       </c>
@@ -998,7 +1021,7 @@
       <c r="G2" s="25"/>
       <c r="H2" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>33</v>
       </c>
@@ -1010,7 +1033,7 @@
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1020,7 +1043,7 @@
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1030,7 +1053,7 @@
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1042,7 +1065,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
@@ -1062,7 +1085,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="30" t="s">
         <v>39</v>
@@ -1086,7 +1109,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="33" t="s">
         <v>46</v>
@@ -1104,13 +1127,13 @@
         <v>0.5</v>
       </c>
       <c r="G9" s="35">
-        <v>1.3322676295501878e-15</v>
+        <v>1.3322676295501878E-15</v>
       </c>
       <c r="H9" s="34">
-        <v>1e+30</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="33" t="s">
         <v>48</v>
@@ -1122,19 +1145,19 @@
         <v>0</v>
       </c>
       <c r="E10" s="35">
-        <v>1.3322676295501878e-15</v>
+        <v>1.3322676295501878E-15</v>
       </c>
       <c r="F10" s="35">
-        <v>0.6000000000000001</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="G10" s="34">
-        <v>1e+30</v>
+        <v>1E+30</v>
       </c>
       <c r="H10" s="35">
-        <v>1.3322676295501878e-15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+        <v>1.3322676295501878E-15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="33" t="s">
         <v>50</v>
@@ -1146,19 +1169,19 @@
         <v>0</v>
       </c>
       <c r="E11" s="35">
-        <v>0.09999999999999876</v>
+        <v>9.9999999999998757E-2</v>
       </c>
       <c r="F11" s="35">
-        <v>0.6499999999999999</v>
+        <v>0.64999999999999991</v>
       </c>
       <c r="G11" s="34">
-        <v>1e+30</v>
+        <v>1E+30</v>
       </c>
       <c r="H11" s="35">
-        <v>0.09999999999999876</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+        <v>9.9999999999998757E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="33" t="s">
         <v>52</v>
@@ -1173,16 +1196,16 @@
         <v>0</v>
       </c>
       <c r="F12" s="35">
-        <v>0.6499999999999999</v>
+        <v>0.64999999999999991</v>
       </c>
       <c r="G12" s="35">
-        <v>0.07999999999999874</v>
+        <v>7.9999999999998739E-2</v>
       </c>
       <c r="H12" s="34">
-        <v>1e+30</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="33" t="s">
         <v>54</v>
@@ -1197,16 +1220,16 @@
         <v>0</v>
       </c>
       <c r="F13" s="35">
-        <v>0.6299999999999999</v>
+        <v>0.62999999999999989</v>
       </c>
       <c r="G13" s="35">
-        <v>0.050000000000001155</v>
+        <v>5.0000000000001155E-2</v>
       </c>
       <c r="H13" s="35">
-        <v>0.07999999999999874</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+        <v>7.9999999999998739E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="33" t="s">
         <v>56</v>
@@ -1218,19 +1241,19 @@
         <v>0</v>
       </c>
       <c r="E14" s="35">
-        <v>0.050000000000001155</v>
+        <v>5.0000000000001155E-2</v>
       </c>
       <c r="F14" s="35">
         <v>0.7799999999999998</v>
       </c>
       <c r="G14" s="34">
-        <v>1e+30</v>
+        <v>1E+30</v>
       </c>
       <c r="H14" s="35">
-        <v>0.050000000000001155</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+        <v>5.0000000000001155E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="33" t="s">
         <v>58</v>
@@ -1251,10 +1274,10 @@
         <v>0.29999999999999893</v>
       </c>
       <c r="H15" s="35">
-        <v>1.13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="33" t="s">
         <v>60</v>
@@ -1278,7 +1301,7 @@
         <v>1.0300000000000002</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="33" t="s">
         <v>62</v>
@@ -1293,16 +1316,16 @@
         <v>0</v>
       </c>
       <c r="F17" s="35">
-        <v>0.2999999999999998</v>
+        <v>0.29999999999999982</v>
       </c>
       <c r="G17" s="35">
-        <v>1.3322676295501878e-15</v>
+        <v>1.3322676295501878E-15</v>
       </c>
       <c r="H17" s="35">
-        <v>0.07999999999999874</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+        <v>7.9999999999998739E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="33" t="s">
         <v>64</v>
@@ -1320,13 +1343,13 @@
         <v>0.5</v>
       </c>
       <c r="G18" s="35">
-        <v>0.09999999999999876</v>
+        <v>9.9999999999998757E-2</v>
       </c>
       <c r="H18" s="35">
-        <v>1.13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="33" t="s">
         <v>66</v>
@@ -1338,19 +1361,19 @@
         <v>0</v>
       </c>
       <c r="E19" s="35">
-        <v>0.07000000000000206</v>
+        <v>7.0000000000002061E-2</v>
       </c>
       <c r="F19" s="35">
-        <v>0.7199999999999998</v>
+        <v>0.71999999999999975</v>
       </c>
       <c r="G19" s="34">
-        <v>1e+30</v>
+        <v>1E+30</v>
       </c>
       <c r="H19" s="35">
-        <v>0.07000000000000206</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+        <v>7.0000000000002061E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="33" t="s">
         <v>68</v>
@@ -1365,16 +1388,16 @@
         <v>0.29999999999999893</v>
       </c>
       <c r="F20" s="35">
-        <v>0.7000000000000002</v>
+        <v>0.70000000000000018</v>
       </c>
       <c r="G20" s="34">
-        <v>1e+30</v>
+        <v>1E+30</v>
       </c>
       <c r="H20" s="35">
         <v>0.29999999999999893</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row r="21" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="33" t="s">
         <v>70</v>
@@ -1389,16 +1412,16 @@
         <v>0.29999999999999805</v>
       </c>
       <c r="F21" s="35">
-        <v>0.5999999999999996</v>
+        <v>0.59999999999999964</v>
       </c>
       <c r="G21" s="34">
-        <v>1e+30</v>
+        <v>1E+30</v>
       </c>
       <c r="H21" s="35">
         <v>0.29999999999999805</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row r="22" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="33" t="s">
         <v>72</v>
@@ -1416,13 +1439,13 @@
         <v>0.20000000000000107</v>
       </c>
       <c r="G22" s="35">
-        <v>0.07999999999999874</v>
+        <v>7.9999999999998739E-2</v>
       </c>
       <c r="H22" s="35">
-        <v>1.3322676295501878e-15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+        <v>1.3322676295501878E-15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="33" t="s">
         <v>74</v>
@@ -1434,19 +1457,19 @@
         <v>0</v>
       </c>
       <c r="E23" s="35">
-        <v>0.09999999999999876</v>
+        <v>9.9999999999998757E-2</v>
       </c>
       <c r="F23" s="35">
         <v>0.5</v>
       </c>
       <c r="G23" s="34">
-        <v>1e+30</v>
+        <v>1E+30</v>
       </c>
       <c r="H23" s="35">
-        <v>0.09999999999999876</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+        <v>9.9999999999998757E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="36" t="s">
         <v>76</v>
@@ -1461,16 +1484,16 @@
         <v>0</v>
       </c>
       <c r="F24" s="38">
-        <v>0.5499999999999989</v>
+        <v>0.54999999999999893</v>
       </c>
       <c r="G24" s="38">
-        <v>0.07000000000000206</v>
+        <v>7.0000000000002061E-2</v>
       </c>
       <c r="H24" s="38">
         <v>1.2799999999999976</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row r="25" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1480,7 +1503,7 @@
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row r="26" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>78</v>
       </c>
@@ -1492,7 +1515,7 @@
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row r="27" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
@@ -1512,7 +1535,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row r="28" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="30" t="s">
         <v>39</v>
@@ -1536,7 +1559,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row r="29" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="33" t="s">
         <v>83</v>
@@ -1548,7 +1571,7 @@
         <v>5000</v>
       </c>
       <c r="E29" s="35">
-        <v>1.13</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="F29" s="34">
         <v>5000</v>
@@ -1560,7 +1583,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row r="30" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="33" t="s">
         <v>85</v>
@@ -1584,7 +1607,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="33" t="s">
         <v>87</v>
@@ -1596,7 +1619,7 @@
         <v>6000</v>
       </c>
       <c r="E31" s="35">
-        <v>0.9299999999999997</v>
+        <v>0.92999999999999972</v>
       </c>
       <c r="F31" s="34">
         <v>6000</v>
@@ -1608,7 +1631,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row r="32" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="33" t="s">
         <v>89</v>
@@ -1620,7 +1643,7 @@
         <v>5500</v>
       </c>
       <c r="E32" s="35">
-        <v>1.13</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="F32" s="34">
         <v>5500</v>
@@ -1632,7 +1655,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row r="33" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="33" t="s">
         <v>91</v>
@@ -1656,7 +1679,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row r="34" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="33" t="s">
         <v>93</v>
@@ -1668,7 +1691,7 @@
         <v>10000</v>
       </c>
       <c r="E34" s="35">
-        <v>-0.1299999999999999</v>
+        <v>-0.12999999999999989</v>
       </c>
       <c r="F34" s="34">
         <v>10000</v>
@@ -1680,7 +1703,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row r="35" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="33" t="s">
         <v>95</v>
@@ -1692,7 +1715,7 @@
         <v>11000</v>
       </c>
       <c r="E35" s="35">
-        <v>-0.07999999999999874</v>
+        <v>-7.9999999999998739E-2</v>
       </c>
       <c r="F35" s="34">
         <v>11000</v>
@@ -1704,7 +1727,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row r="36" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="33" t="s">
         <v>97</v>
@@ -1722,13 +1745,13 @@
         <v>10500</v>
       </c>
       <c r="G36" s="34">
-        <v>1e+30</v>
+        <v>1E+30</v>
       </c>
       <c r="H36" s="34">
         <v>1250</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row r="37" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="33" t="s">
         <v>99</v>
@@ -1740,7 +1763,7 @@
         <v>19250</v>
       </c>
       <c r="E37" s="35">
-        <v>0.6299999999999999</v>
+        <v>0.62999999999999989</v>
       </c>
       <c r="F37" s="34">
         <v>0</v>
@@ -1752,7 +1775,7 @@
         <v>9250</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row r="38" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="36" t="s">
         <v>101</v>
@@ -1764,7 +1787,7 @@
         <v>11000</v>
       </c>
       <c r="E38" s="38">
-        <v>0.7299999999999986</v>
+        <v>0.72999999999999865</v>
       </c>
       <c r="F38" s="37">
         <v>0</v>
@@ -1782,31 +1805,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView zoomScale="208" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
@@ -1824,7 +1843,7 @@
       <c r="K1" s="7"/>
       <c r="L1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
         <v>14</v>
@@ -1846,7 +1865,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>7</v>
@@ -1868,7 +1887,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
         <v>8</v>
@@ -1890,7 +1909,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
         <v>9</v>
@@ -1912,7 +1931,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="2"/>
@@ -1926,7 +1945,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row r="7" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
@@ -1942,7 +1961,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
         <v>16</v>
@@ -1968,7 +1987,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row r="9" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
         <v>10</v>
@@ -1994,7 +2013,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row r="10" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7" t="s">
         <v>11</v>
@@ -2012,7 +2031,7 @@
         <v>0.5</v>
       </c>
       <c r="G10" s="11">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -2020,7 +2039,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row r="11" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7" t="s">
         <v>0</v>
@@ -2046,7 +2065,7 @@
       <c r="K11" s="7"/>
       <c r="L11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row r="12" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="2"/>
@@ -2060,7 +2079,7 @@
       <c r="K12" s="7"/>
       <c r="L12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row r="13" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>17</v>
       </c>
@@ -2076,7 +2095,7 @@
       <c r="K13" s="7"/>
       <c r="L13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row r="14" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="2" t="s">
@@ -2092,7 +2111,7 @@
       <c r="K14" s="7"/>
       <c r="L14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row r="15" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
         <v>14</v>
@@ -2116,7 +2135,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row r="16" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
         <v>7</v>
@@ -2129,6 +2148,7 @@
       </c>
       <c r="E16" s="17">
         <f>SUM(C16:D16)</f>
+        <v>10000</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>20</v>
@@ -2142,7 +2162,7 @@
       <c r="K16" s="7"/>
       <c r="L16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row r="17" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
         <v>8</v>
@@ -2155,6 +2175,7 @@
       </c>
       <c r="E17" s="17">
         <f>SUM(C17:D17)</f>
+        <v>11000</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>20</v>
@@ -2168,7 +2189,7 @@
       <c r="K17" s="7"/>
       <c r="L17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row r="18" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
         <v>9</v>
@@ -2181,6 +2202,7 @@
       </c>
       <c r="E18" s="17">
         <f>SUM(C18:D18)</f>
+        <v>9250</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>20</v>
@@ -2194,7 +2216,7 @@
       <c r="K18" s="7"/>
       <c r="L18" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row r="19" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="2"/>
@@ -2208,7 +2230,7 @@
       <c r="K19" s="7"/>
       <c r="L19" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row r="20" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="2" t="s">
@@ -2224,7 +2246,7 @@
       <c r="K20" s="7"/>
       <c r="L20" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row r="21" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
         <v>16</v>
@@ -2252,7 +2274,7 @@
       <c r="K21" s="7"/>
       <c r="L21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row r="22" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="7" t="s">
         <v>10</v>
@@ -2280,7 +2302,7 @@
       <c r="K22" s="7"/>
       <c r="L22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row r="23" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7" t="s">
         <v>11</v>
@@ -2310,25 +2332,30 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row r="24" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="17">
         <f>SUM(C22:C23)</f>
+        <v>5000</v>
       </c>
       <c r="D24" s="17">
         <f>SUM(D22:D23)</f>
+        <v>7500</v>
       </c>
       <c r="E24" s="17">
         <f>SUM(E22:E23)</f>
+        <v>6000</v>
       </c>
       <c r="F24" s="17">
         <f>SUM(F22:F23)</f>
+        <v>5500</v>
       </c>
       <c r="G24" s="17">
         <f>SUM(G22:G23)</f>
+        <v>6250</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7" t="s">
@@ -2336,15 +2363,17 @@
       </c>
       <c r="J24" s="17">
         <f>SUM(C16:C18)</f>
+        <v>19250</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>25</v>
       </c>
       <c r="L24" s="17">
         <f>SUM(C22:G22)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+        <v>19250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="20" t="s">
@@ -2368,15 +2397,17 @@
       </c>
       <c r="J25" s="17">
         <f>SUM(D16:D18)</f>
+        <v>11000</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>25</v>
       </c>
       <c r="L25" s="17">
         <f>SUM(C23:G23)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="7" t="s">
         <v>19</v>
@@ -2402,7 +2433,7 @@
       <c r="K26" s="7"/>
       <c r="L26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row r="27" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="2"/>
@@ -2416,7 +2447,7 @@
       <c r="K27" s="7"/>
       <c r="L27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row r="28" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="2"/>
@@ -2436,7 +2467,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row r="29" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
         <v>30</v>
       </c>
@@ -2445,12 +2476,15 @@
       <c r="D29" s="2"/>
       <c r="E29" s="22">
         <f>SUMPRODUCT(C3:D5,C16:D18)</f>
+        <v>17977.5</v>
       </c>
       <c r="F29" s="22">
         <f>SUMPRODUCT(C9:G10,C22:G23)</f>
+        <v>13012.5</v>
       </c>
       <c r="G29" s="23">
         <f>SUM(E29:F29)</f>
+        <v>30990</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -2464,53 +2498,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A2:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="255" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="12.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="10" t="s">
+    <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="11">
-        <v>0.6</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="7"/>
@@ -2520,15 +2531,15 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="11">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="C3" s="11">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="7"/>
@@ -2538,28 +2549,34 @@
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.65</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.65</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B5" s="11">
         <v>0.63</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C5" s="11">
         <v>0.78</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2568,7 +2585,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
@@ -2580,13 +2597,25 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
+    <row r="7" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2594,17 +2623,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="12.5" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
       <c r="B1" s="10" t="s">
         <v>1</v>
@@ -2622,7 +2647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -2642,7 +2667,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -2659,7 +2684,7 @@
         <v>0.5</v>
       </c>
       <c r="F3" s="11">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -2668,7 +2693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2676,15 +2701,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -2692,7 +2716,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -2702,7 +2726,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -2712,7 +2736,7 @@
       <c r="C3" s="3"/>
       <c r="D3" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
@@ -2722,13 +2746,13 @@
       <c r="C4" s="3"/>
       <c r="D4" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="8"/>
       <c r="C5" s="3"/>
       <c r="D5" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="8"/>
       <c r="C6" s="3"/>
@@ -2740,7 +2764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2748,19 +2772,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2768,7 +2792,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2776,7 +2800,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2784,7 +2808,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2792,7 +2816,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>